<commit_message>
redmine #9280 cal sheets added/modified in repo for CP05MOAS gliders 335, 336, 339, 340, 374, 375, 376 multiple deployments.
</commit_message>
<xml_diff>
--- a/CP05MOAS-GL335/Omaha_Cal_Info_CP05MOAS-GL335_00001.xlsx
+++ b/CP05MOAS-GL335/Omaha_Cal_Info_CP05MOAS-GL335_00001.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19830" windowHeight="8055" tabRatio="377"/>
+    <workbookView xWindow="140" yWindow="180" windowWidth="23140" windowHeight="7960" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,12 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$103</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$376</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -103,18 +108,9 @@
     <t>Anchor Launch Date</t>
   </si>
   <si>
-    <t>70°35.0053'W</t>
-  </si>
-  <si>
-    <t>39°49.7765'N</t>
-  </si>
-  <si>
     <t>KN-222</t>
   </si>
   <si>
-    <t>EB</t>
-  </si>
-  <si>
     <t>Mooring Serial Number</t>
   </si>
   <si>
@@ -137,6 +133,15 @@
   </si>
   <si>
     <t>CP05MOAS-GL335-00-ENG000000</t>
+  </si>
+  <si>
+    <t>39° 50' N</t>
+  </si>
+  <si>
+    <t>70° 42.5' W</t>
+  </si>
+  <si>
+    <t>EB Line</t>
   </si>
 </sst>
 </file>
@@ -220,12 +225,11 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,18 +244,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -313,13 +311,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -365,9 +376,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -379,11 +387,17 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="8" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="11" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -760,26 +774,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="37.85546875"/>
-    <col min="2" max="2" width="39.42578125"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.42578125"/>
-    <col min="7" max="7" width="18.7109375"/>
-    <col min="8" max="8" width="18.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875"/>
-    <col min="10" max="10" width="12.7109375"/>
-    <col min="11" max="11" width="51.7109375"/>
-    <col min="12" max="1026" width="8.7109375"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="8" width="17" customWidth="1"/>
+    <col min="9" max="10" width="11.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -814,9 +822,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="10" customFormat="1" ht="15">
       <c r="A2" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" s="11">
         <v>335</v>
@@ -830,46 +838,51 @@
       <c r="E2" s="13">
         <v>0.63055555555555554</v>
       </c>
-      <c r="F2" s="25">
-        <v>42016</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="19" t="s">
+      <c r="F2" s="26">
+        <v>41988</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="28">
+        <v>200</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="11">
-        <v>0</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>24</v>
-      </c>
       <c r="K2" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="23">
+        <v>33</v>
+      </c>
+      <c r="L2" s="22">
         <f>((LEFT(G2,(FIND("°",G2,1)-1)))+(MID(G2,(FIND("°",G2,1)+1),(FIND("'",G2,1))-(FIND("°",G2,1)+1))/60))*(IF(RIGHT(G2,1)="N",1,-1))</f>
-        <v>39.829608333333333</v>
-      </c>
-      <c r="M2" s="23">
+        <v>39.833333333333336</v>
+      </c>
+      <c r="M2" s="22">
         <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="E",1,-1))</f>
-        <v>-70.583421666666666</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>-70.708333333333329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="5"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -877,30 +890,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125"/>
-    <col min="8" max="8" width="11.85546875"/>
-    <col min="9" max="9" width="14.42578125"/>
-    <col min="10" max="10" width="13.42578125"/>
-    <col min="11" max="1025" width="8.7109375"/>
+    <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="28.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>11</v>
@@ -915,9 +923,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" s="17">
         <v>335</v>
@@ -925,29 +933,29 @@
       <c r="C2" s="17">
         <v>1</v>
       </c>
-      <c r="D2" s="22">
+      <c r="D2" s="21">
         <v>643111</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="24">
+      <c r="F2" s="23">
         <v>0.61</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3" s="17">
         <v>335</v>
@@ -955,29 +963,29 @@
       <c r="C3" s="17">
         <v>1</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="21">
         <v>643111</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="23">
         <v>0.61</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" s="17">
         <v>335</v>
@@ -985,29 +993,29 @@
       <c r="C4" s="17">
         <v>1</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="21">
         <v>643111</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="23">
         <v>0.61</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B5" s="17">
         <v>335</v>
@@ -1015,47 +1023,47 @@
       <c r="C5" s="17">
         <v>1</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="21">
         <v>643111</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="23">
         <v>0.61</v>
       </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="9"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
-      <c r="D6" s="22"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="18"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-    </row>
-    <row r="7" spans="1:16" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F6" s="23"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+    </row>
+    <row r="7" spans="1:16" s="8" customFormat="1">
       <c r="A7" s="14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B7" s="17">
         <v>335</v>
@@ -1063,13 +1071,13 @@
       <c r="C7" s="17">
         <v>1</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="21">
         <v>2809</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="25">
         <v>124</v>
       </c>
       <c r="G7" s="15"/>
@@ -1078,9 +1086,9 @@
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
     </row>
-    <row r="8" spans="1:16" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" s="8" customFormat="1">
       <c r="A8" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B8" s="17">
         <v>335</v>
@@ -1088,13 +1096,13 @@
       <c r="C8" s="17">
         <v>1</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="21">
         <v>2809</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="24">
         <v>700</v>
       </c>
       <c r="G8" s="15"/>
@@ -1103,9 +1111,9 @@
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
     </row>
-    <row r="9" spans="1:16" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" s="8" customFormat="1">
       <c r="A9" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B9" s="17">
         <v>335</v>
@@ -1113,13 +1121,13 @@
       <c r="C9" s="17">
         <v>1</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="21">
         <v>2809</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="25">
         <v>1.0760000000000001</v>
       </c>
       <c r="G9" s="15"/>
@@ -1128,9 +1136,9 @@
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
     </row>
-    <row r="10" spans="1:16" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" s="8" customFormat="1">
       <c r="A10" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B10" s="17">
         <v>335</v>
@@ -1138,13 +1146,13 @@
       <c r="C10" s="17">
         <v>1</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="21">
         <v>2809</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="24">
         <v>3.9E-2</v>
       </c>
       <c r="G10" s="15"/>
@@ -1153,22 +1161,22 @@
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
     </row>
-    <row r="11" spans="1:16" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" s="8" customFormat="1">
       <c r="A11" s="9"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="26"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="24"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
     </row>
-    <row r="12" spans="1:16" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" s="8" customFormat="1">
       <c r="A12" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B12" s="17">
         <v>335</v>
@@ -1176,7 +1184,7 @@
       <c r="C12" s="17">
         <v>1</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="21">
         <v>9029</v>
       </c>
       <c r="E12" s="15"/>
@@ -1187,11 +1195,11 @@
       <c r="J12" s="15"/>
       <c r="K12" s="15"/>
     </row>
-    <row r="13" spans="1:16" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" s="8" customFormat="1">
       <c r="A13" s="14"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
-      <c r="D13" s="22"/>
+      <c r="D13" s="21"/>
       <c r="E13" s="15"/>
       <c r="F13" s="16"/>
       <c r="G13" s="15"/>
@@ -1200,9 +1208,9 @@
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
     </row>
-    <row r="14" spans="1:16" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" s="8" customFormat="1">
       <c r="A14" s="14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B14" s="17">
         <v>335</v>
@@ -1210,7 +1218,7 @@
       <c r="C14" s="17">
         <v>1</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="21">
         <v>105</v>
       </c>
       <c r="E14" s="15"/>
@@ -1221,11 +1229,11 @@
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
     </row>
-    <row r="15" spans="1:16" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" s="8" customFormat="1">
       <c r="A15" s="14"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
-      <c r="D15" s="22"/>
+      <c r="D15" s="21"/>
       <c r="E15" s="15"/>
       <c r="F15" s="16"/>
       <c r="G15" s="15"/>
@@ -1234,9 +1242,9 @@
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
     </row>
-    <row r="16" spans="1:16" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" s="8" customFormat="1">
       <c r="A16" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B16" s="17">
         <v>335</v>
@@ -1244,7 +1252,7 @@
       <c r="C16" s="17">
         <v>1</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="21">
         <v>50151</v>
       </c>
       <c r="E16" s="15"/>
@@ -1255,11 +1263,11 @@
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" s="8" customFormat="1">
       <c r="A17" s="14"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
-      <c r="D17" s="22"/>
+      <c r="D17" s="21"/>
       <c r="E17" s="15"/>
       <c r="F17" s="16"/>
       <c r="G17" s="15"/>
@@ -1268,9 +1276,9 @@
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
     </row>
-    <row r="18" spans="1:11" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" s="8" customFormat="1">
       <c r="A18" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B18" s="17">
         <v>335</v>
@@ -1278,7 +1286,7 @@
       <c r="C18" s="17">
         <v>1</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="21">
         <v>335</v>
       </c>
       <c r="E18" s="15"/>
@@ -1289,7 +1297,7 @@
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
     </row>
-    <row r="19" spans="1:11" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="8" customFormat="1">
       <c r="A19" s="15"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
@@ -1304,6 +1312,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>